<commit_message>
done pipeline running on any cell definition. ready to match with matan version
</commit_message>
<xml_diff>
--- a/Data/division_choice/20/cell2name.xlsx
+++ b/Data/division_choice/20/cell2name.xlsx
@@ -39,9 +39,6 @@
     <t>62_arab</t>
   </si>
   <si>
-    <t>Jerusalem &amp; suburbs</t>
-  </si>
-  <si>
     <t>Bet Shemesh</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>Kinneret</t>
   </si>
   <si>
-    <t>Yizreel</t>
-  </si>
-  <si>
     <t>Akko</t>
   </si>
   <si>
@@ -78,25 +72,31 @@
     <t>Rehovot</t>
   </si>
   <si>
-    <t>Tel Aviv city</t>
-  </si>
-  <si>
-    <t>Tel Aviv suburbs</t>
-  </si>
-  <si>
-    <t>Bene Beraq</t>
-  </si>
-  <si>
     <t>Ashqelon</t>
   </si>
   <si>
     <t>Beer Sheva Jewish</t>
   </si>
   <si>
-    <t>Beer Sheva Arab</t>
-  </si>
-  <si>
     <t>Judea and Samaria</t>
+  </si>
+  <si>
+    <t>TLV suburbs</t>
+  </si>
+  <si>
+    <t>Bnei Brak</t>
+  </si>
+  <si>
+    <t>Tel Aviv - Yafo</t>
+  </si>
+  <si>
+    <t>Jerusalem and sub.</t>
+  </si>
+  <si>
+    <t>Jezreel Valley</t>
+  </si>
+  <si>
+    <t>Beer Sheva Arabs</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <dimension ref="A1:B251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B21"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -468,7 +468,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -476,7 +476,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -484,7 +484,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -492,7 +492,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -500,7 +500,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -508,7 +508,7 @@
         <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -516,7 +516,7 @@
         <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -524,7 +524,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -532,7 +532,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -540,7 +540,7 @@
         <v>41</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -548,7 +548,7 @@
         <v>42</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -556,7 +556,7 @@
         <v>43</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -564,7 +564,7 @@
         <v>44</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -572,7 +572,7 @@
         <v>51</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -596,7 +596,7 @@
         <v>61</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -604,7 +604,7 @@
         <v>62</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -612,7 +612,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -620,7 +620,7 @@
         <v>71</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>